<commit_message>
Change scripts and files
</commit_message>
<xml_diff>
--- a/01.04.19_MTT_Perkin_data/final_data/combined_finale_data.xlsx
+++ b/01.04.19_MTT_Perkin_data/final_data/combined_finale_data.xlsx
@@ -1054,18 +1054,73 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1074,11 +1129,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1382,1352 +1450,1368 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="8.88671875" style="7"/>
+    <col min="10" max="10" width="8.88671875" style="5"/>
+    <col min="11" max="17" width="8.88671875" style="6"/>
+    <col min="18" max="18" width="8.88671875" style="7"/>
+    <col min="19" max="19" width="8.88671875" style="5"/>
+    <col min="20" max="26" width="8.88671875" style="6"/>
+    <col min="27" max="27" width="8.88671875" style="7"/>
+    <col min="28" max="28" width="8.88671875" style="5"/>
+    <col min="29" max="35" width="8.88671875" style="6"/>
+    <col min="36" max="36" width="8.88671875" style="7"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AB2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="N3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="W3" t="s">
-        <v>17</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="W3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AB3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AF3" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG3" t="s">
+      <c r="AF3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AH3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AI3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AJ3" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="N4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="N4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="W4" t="s">
-        <v>17</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="W4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X4" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Y4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AA4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AB4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AC4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AF4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG4" t="s">
+      <c r="AF4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AH4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AI4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AJ4" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="N5" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="N5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="W5" t="s">
-        <v>17</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="W5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X5" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Y5" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="Z5" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AA5" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AB5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AC5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AF5" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AG5" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AH5" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AI5" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AJ5" s="7" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="N6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="N6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="U6" t="s">
+      <c r="U6" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="V6" t="s">
+      <c r="V6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="W6" t="s">
+      <c r="W6" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="X6" t="s">
+      <c r="X6" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Y6" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="Z6" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AA6" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AB6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AC6" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD6" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AE6" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AF6" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AG6" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AH6" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AI6" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AJ6" s="7" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="W7" t="s">
+      <c r="W7" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="X7" t="s">
+      <c r="X7" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Y7" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="Z7" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AA7" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AB7" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AC7" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="AF7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG7" t="s">
+      <c r="AF7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG7" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AH7" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AI7" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AJ7" s="7" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="N8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="N8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S8" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="W8" t="s">
-        <v>17</v>
-      </c>
-      <c r="X8" t="s">
+      <c r="W8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X8" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Y8" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="Z8" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AA8" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AB8" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AC8" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AD8" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AE8" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="AF8" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG8" t="s">
+      <c r="AF8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG8" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AH8" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AI8" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="AJ8" t="s">
+      <c r="AJ8" s="7" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V9" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W9" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="X9" t="s">
+      <c r="X9" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Y9" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="Z9" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AA9" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AB9" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AC9" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AD9" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AE9" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AF9" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AG9" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AH9" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AI9" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AJ9" s="7" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S10" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U10" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="V10" t="s">
+      <c r="V10" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="W10" t="s">
+      <c r="W10" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="X10" t="s">
+      <c r="X10" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Y10" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="Z10" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AA10" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AB10" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AC10" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AD10" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AE10" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AF10" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AG10" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AH10" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AI10" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="AJ10" t="s">
+      <c r="AJ10" s="7" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="N11" t="s">
-        <v>17</v>
-      </c>
-      <c r="O11" t="s">
+      <c r="N11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S11" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="X11" t="s">
+      <c r="X11" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Y11" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="Z11" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AA11" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AB11" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AC11" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="AF11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG11" t="s">
+      <c r="AF11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG11" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AH11" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AI11" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="AJ11" t="s">
+      <c r="AJ11" s="7" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="N12" t="s">
-        <v>17</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="N12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="U12" t="s">
+      <c r="U12" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="V12" t="s">
+      <c r="V12" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="W12" t="s">
-        <v>17</v>
-      </c>
-      <c r="X12" t="s">
+      <c r="W12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X12" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Y12" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="Z12" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AA12" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AB12" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AC12" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AD12" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AE12" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="AF12" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG12" t="s">
+      <c r="AF12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG12" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AH12" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AI12" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AJ12" s="7" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="N13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="N13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W13" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="X13" t="s">
+      <c r="X13" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Y13" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="Z13" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AA13" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AB13" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AC13" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="AF13" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG13" t="s">
+      <c r="AF13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG13" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="AH13" t="s">
+      <c r="AH13" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AI13" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AJ13" s="7" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="N14" t="s">
-        <v>17</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="N14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q14" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S14" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="U14" t="s">
+      <c r="U14" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="V14" t="s">
+      <c r="V14" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="W14" t="s">
-        <v>17</v>
-      </c>
-      <c r="X14" t="s">
+      <c r="W14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X14" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Y14" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="Z14" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AA14" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AB14" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AC14" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AD14" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AE14" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="AF14" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG14" t="s">
+      <c r="AF14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG14" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AH14" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AI14" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="AJ14" t="s">
+      <c r="AJ14" s="7" t="s">
         <v>338</v>
       </c>
     </row>

</xml_diff>

<commit_message>
# Move scripts to the separate folder
</commit_message>
<xml_diff>
--- a/01.04.19_MTT_Perkin_data/final_data/combined_finale_data.xlsx
+++ b/01.04.19_MTT_Perkin_data/final_data/combined_finale_data.xlsx
@@ -1037,7 +1037,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1049,6 +1049,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1129,7 +1136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1147,6 +1154,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1451,7 +1462,7 @@
   <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1467,7 +1478,7 @@
     <col min="27" max="27" width="8.88671875" style="7"/>
     <col min="28" max="28" width="8.88671875" style="5"/>
     <col min="29" max="35" width="8.88671875" style="6"/>
-    <col min="36" max="36" width="8.88671875" style="7"/>
+    <col min="36" max="36" width="20.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1634,7 +1645,7 @@
       <c r="M3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O3" s="6" t="s">
@@ -1661,7 +1672,7 @@
       <c r="V3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="X3" s="6" t="s">
@@ -1682,7 +1693,7 @@
       <c r="AC3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AF3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="AG3" s="6" t="s">
@@ -1738,7 +1749,7 @@
       <c r="M4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O4" s="6" t="s">
@@ -1765,7 +1776,7 @@
       <c r="V4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="W4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="X4" s="6" t="s">
@@ -1786,7 +1797,7 @@
       <c r="AC4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AF4" s="6" t="s">
+      <c r="AF4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="AG4" s="6" t="s">
@@ -1836,7 +1847,7 @@
       <c r="M5" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O5" s="6" t="s">
@@ -1857,7 +1868,7 @@
       <c r="T5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="W5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="X5" s="6" t="s">
@@ -1878,19 +1889,19 @@
       <c r="AC5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AF5" s="6" t="s">
+      <c r="AF5" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="AG5" s="6" t="s">
+      <c r="AG5" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="AH5" s="6" t="s">
+      <c r="AH5" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AI5" s="6" t="s">
+      <c r="AI5" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="AJ5" s="7" t="s">
+      <c r="AJ5" s="9" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1934,7 +1945,7 @@
       <c r="M6" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O6" s="6" t="s">
@@ -1961,19 +1972,19 @@
       <c r="V6" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="W6" s="6" t="s">
+      <c r="W6" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="X6" s="6" t="s">
+      <c r="X6" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="Y6" s="6" t="s">
+      <c r="Y6" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="Z6" s="6" t="s">
+      <c r="Z6" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="AA6" s="7" t="s">
+      <c r="AA6" s="9" t="s">
         <v>113</v>
       </c>
       <c r="AB6" s="5" t="s">
@@ -1988,19 +1999,19 @@
       <c r="AE6" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="AF6" s="6" t="s">
+      <c r="AF6" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="AG6" s="6" t="s">
+      <c r="AG6" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="AH6" s="6" t="s">
+      <c r="AH6" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="AI6" s="6" t="s">
+      <c r="AI6" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="AJ6" s="7" t="s">
+      <c r="AJ6" s="9" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2020,16 +2031,16 @@
       <c r="E7" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="9" t="s">
         <v>130</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -2044,7 +2055,7 @@
       <c r="M7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N7" s="8" t="s">
         <v>133</v>
       </c>
       <c r="O7" s="6" t="s">
@@ -2065,19 +2076,19 @@
       <c r="T7" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="W7" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="X7" s="6" t="s">
+      <c r="X7" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="Y7" s="6" t="s">
+      <c r="Y7" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Z7" s="6" t="s">
+      <c r="Z7" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="AA7" s="7" t="s">
+      <c r="AA7" s="9" t="s">
         <v>143</v>
       </c>
       <c r="AB7" s="5" t="s">
@@ -2086,7 +2097,7 @@
       <c r="AC7" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="AF7" s="6" t="s">
+      <c r="AF7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="AG7" s="6" t="s">
@@ -2136,7 +2147,7 @@
       <c r="M8" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O8" s="6" t="s">
@@ -2157,7 +2168,7 @@
       <c r="T8" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="W8" s="6" t="s">
+      <c r="W8" s="8" t="s">
         <v>17</v>
       </c>
       <c r="X8" s="6" t="s">
@@ -2184,19 +2195,19 @@
       <c r="AE8" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="AF8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG8" s="6" t="s">
+      <c r="AF8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG8" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="AH8" s="6" t="s">
+      <c r="AH8" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="AI8" s="6" t="s">
+      <c r="AI8" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="AJ8" s="7" t="s">
+      <c r="AJ8" s="9" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2240,19 +2251,19 @@
       <c r="M9" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="P9" s="6" t="s">
+      <c r="P9" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="Q9" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="R9" s="7" t="s">
+      <c r="R9" s="9" t="s">
         <v>190</v>
       </c>
       <c r="S9" s="5" t="s">
@@ -2267,19 +2278,19 @@
       <c r="V9" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="W9" s="6" t="s">
+      <c r="W9" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="X9" s="6" t="s">
+      <c r="X9" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="Y9" s="6" t="s">
+      <c r="Y9" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="Z9" s="6" t="s">
+      <c r="Z9" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="AA9" s="7" t="s">
+      <c r="AA9" s="9" t="s">
         <v>198</v>
       </c>
       <c r="AB9" s="5" t="s">
@@ -2294,19 +2305,19 @@
       <c r="AE9" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AF9" s="6" t="s">
+      <c r="AF9" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="AG9" s="6" t="s">
+      <c r="AG9" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="AH9" s="6" t="s">
+      <c r="AH9" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="AI9" s="6" t="s">
+      <c r="AI9" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="AJ9" s="7" t="s">
+      <c r="AJ9" s="9" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2326,16 +2337,16 @@
       <c r="E10" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="9" t="s">
         <v>215</v>
       </c>
       <c r="J10" s="5" t="s">
@@ -2350,19 +2361,19 @@
       <c r="M10" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="P10" s="6" t="s">
+      <c r="P10" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="R10" s="7" t="s">
+      <c r="R10" s="9" t="s">
         <v>223</v>
       </c>
       <c r="S10" s="5" t="s">
@@ -2377,25 +2388,25 @@
       <c r="V10" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="W10" s="6" t="s">
+      <c r="W10" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="X10" s="6" t="s">
+      <c r="X10" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="Y10" s="6" t="s">
+      <c r="Y10" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="Z10" s="6" t="s">
+      <c r="Z10" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="AA10" s="7" t="s">
+      <c r="AA10" s="9" t="s">
         <v>231</v>
       </c>
       <c r="AB10" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="AC10" s="6" t="s">
+      <c r="AC10" s="8" t="s">
         <v>232</v>
       </c>
       <c r="AD10" s="6" t="s">
@@ -2404,10 +2415,10 @@
       <c r="AE10" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="AF10" s="6" t="s">
+      <c r="AF10" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="AG10" s="6" t="s">
+      <c r="AG10" s="8" t="s">
         <v>236</v>
       </c>
       <c r="AH10" s="6" t="s">
@@ -2445,7 +2456,7 @@
       <c r="K11" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="N11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O11" s="6" t="s">
@@ -2466,19 +2477,19 @@
       <c r="T11" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="W11" s="6" t="s">
+      <c r="W11" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="X11" s="6" t="s">
+      <c r="X11" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="Y11" s="6" t="s">
+      <c r="Y11" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="Z11" s="6" t="s">
+      <c r="Z11" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="AA11" s="7" t="s">
+      <c r="AA11" s="9" t="s">
         <v>254</v>
       </c>
       <c r="AB11" s="5" t="s">
@@ -2487,19 +2498,19 @@
       <c r="AC11" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="AF11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG11" s="6" t="s">
+      <c r="AF11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG11" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="AH11" s="6" t="s">
+      <c r="AH11" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="AI11" s="6" t="s">
+      <c r="AI11" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="AJ11" s="7" t="s">
+      <c r="AJ11" s="11" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2537,7 +2548,7 @@
       <c r="M12" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O12" s="6" t="s">
@@ -2564,7 +2575,7 @@
       <c r="V12" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="W12" s="6" t="s">
+      <c r="W12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="X12" s="6" t="s">
@@ -2591,7 +2602,7 @@
       <c r="AE12" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="AF12" s="6" t="s">
+      <c r="AF12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="AG12" s="6" t="s">
@@ -2647,7 +2658,7 @@
       <c r="M13" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O13" s="6" t="s">
@@ -2668,19 +2679,19 @@
       <c r="T13" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="W13" s="6" t="s">
+      <c r="W13" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="X13" s="6" t="s">
+      <c r="X13" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="Y13" s="6" t="s">
+      <c r="Y13" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="Z13" s="6" t="s">
+      <c r="Z13" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="AA13" s="7" t="s">
+      <c r="AA13" s="9" t="s">
         <v>305</v>
       </c>
       <c r="AB13" s="5" t="s">
@@ -2689,7 +2700,7 @@
       <c r="AC13" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="AF13" s="6" t="s">
+      <c r="AF13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="AG13" s="6" t="s">
@@ -2745,7 +2756,7 @@
       <c r="M14" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="N14" s="8" t="s">
         <v>17</v>
       </c>
       <c r="O14" s="6" t="s">
@@ -2772,19 +2783,19 @@
       <c r="V14" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="W14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="X14" s="6" t="s">
+      <c r="W14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="X14" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="Y14" s="6" t="s">
+      <c r="Y14" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="Z14" s="6" t="s">
+      <c r="Z14" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="AA14" s="7" t="s">
+      <c r="AA14" s="9" t="s">
         <v>331</v>
       </c>
       <c r="AB14" s="5" t="s">
@@ -2799,7 +2810,7 @@
       <c r="AE14" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="AF14" s="6" t="s">
+      <c r="AF14" s="8" t="s">
         <v>17</v>
       </c>
       <c r="AG14" s="6" t="s">
@@ -2817,5 +2828,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>